<commit_message>
Changement dans l'export Twizzzit Ledger_Account devient Compte général
</commit_message>
<xml_diff>
--- a/RUSConvert/Files/TwizzitInvoicesExport.xlsx
+++ b/RUSConvert/Files/TwizzitInvoicesExport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Documents RUS\REPO\RUSConvert\RUSConvert\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\REPO\rus-convert\RUSConvert\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1FB52F-AAD7-4D08-94C8-A049430C1BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262BDE5E-6557-4816-99F7-52B18476BC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6810" yWindow="2580" windowWidth="42000" windowHeight="15645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="660" windowWidth="18975" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Ledger Account</t>
-  </si>
-  <si>
     <t>Référence</t>
   </si>
   <si>
@@ -357,6 +354,9 @@
   </si>
   <si>
     <t>DEMO Sophie - Cotisation Club</t>
+  </si>
+  <si>
+    <t>Compte général</t>
   </si>
 </sst>
 </file>
@@ -728,7 +728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -812,1861 +814,1861 @@
         <v>24</v>
       </c>
       <c r="AA1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
       <c r="AC1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
         <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
       </c>
       <c r="F2" t="str">
         <f>D2&amp;"    Chaussée de Ruisbroek 18  1180 Uccle Belgique"</f>
         <v>DUPONT    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
         <v>31</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>32</v>
       </c>
-      <c r="I2" t="s">
-        <v>33</v>
-      </c>
       <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
         <v>34</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
         <v>35</v>
       </c>
-      <c r="L2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>36</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>37</v>
       </c>
-      <c r="O2" t="s">
-        <v>38</v>
-      </c>
       <c r="P2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>40</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" t="s">
         <v>41</v>
       </c>
-      <c r="U2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
+        <v>88</v>
+      </c>
+      <c r="X2" t="s">
         <v>42</v>
       </c>
-      <c r="W2" t="s">
-        <v>89</v>
-      </c>
-      <c r="X2" t="s">
-        <v>43</v>
-      </c>
       <c r="Y2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AC2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
         <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F23" si="0">D3&amp;"    Chaussée de Ruisbroek 18  1180 Uccle Belgique"</f>
         <v>DUPONT    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>32</v>
       </c>
-      <c r="I3" t="s">
-        <v>33</v>
-      </c>
       <c r="J3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" t="s">
         <v>34</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s">
         <v>35</v>
       </c>
-      <c r="L3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>36</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>37</v>
       </c>
-      <c r="O3" t="s">
-        <v>38</v>
-      </c>
       <c r="P3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>40</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
+        <v>38</v>
+      </c>
+      <c r="V3" t="s">
         <v>41</v>
       </c>
-      <c r="U3" t="s">
-        <v>39</v>
-      </c>
-      <c r="V3" t="s">
-        <v>42</v>
-      </c>
       <c r="W3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="X3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Y3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AC3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
         <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
         <v>DUPONT    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
         <v>31</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>32</v>
       </c>
-      <c r="I4" t="s">
-        <v>33</v>
-      </c>
       <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
         <v>34</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" t="s">
         <v>35</v>
       </c>
-      <c r="L4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>36</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>37</v>
       </c>
-      <c r="O4" t="s">
-        <v>38</v>
-      </c>
       <c r="P4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" t="s">
         <v>39</v>
       </c>
-      <c r="Q4" t="s">
-        <v>38</v>
-      </c>
-      <c r="R4" t="s">
-        <v>38</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>40</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
+        <v>38</v>
+      </c>
+      <c r="V4" t="s">
         <v>41</v>
       </c>
-      <c r="U4" t="s">
-        <v>39</v>
-      </c>
-      <c r="V4" t="s">
-        <v>42</v>
-      </c>
       <c r="W4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="X4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Y4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AC4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
       <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" t="s">
         <v>46</v>
-      </c>
-      <c r="D5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
         <v>DURANT    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
         <v>31</v>
       </c>
-      <c r="H5" t="s">
-        <v>32</v>
-      </c>
       <c r="I5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" t="s">
         <v>34</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" t="s">
         <v>35</v>
       </c>
-      <c r="L5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>36</v>
       </c>
-      <c r="N5" t="s">
-        <v>37</v>
-      </c>
       <c r="O5" t="s">
+        <v>48</v>
+      </c>
+      <c r="P5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>48</v>
+      </c>
+      <c r="R5" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" t="s">
         <v>49</v>
       </c>
-      <c r="P5" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>49</v>
-      </c>
-      <c r="R5" t="s">
-        <v>49</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>50</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
+        <v>38</v>
+      </c>
+      <c r="V5" t="s">
+        <v>41</v>
+      </c>
+      <c r="W5" t="s">
+        <v>91</v>
+      </c>
+      <c r="X5" t="s">
         <v>51</v>
       </c>
-      <c r="U5" t="s">
-        <v>39</v>
-      </c>
-      <c r="V5" t="s">
-        <v>42</v>
-      </c>
-      <c r="W5" t="s">
-        <v>92</v>
-      </c>
-      <c r="X5" t="s">
-        <v>52</v>
-      </c>
       <c r="Y5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AC5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
       <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" t="s">
         <v>46</v>
-      </c>
-      <c r="D6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" t="s">
-        <v>47</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
         <v>DURANT    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
         <v>31</v>
       </c>
-      <c r="H6" t="s">
-        <v>32</v>
-      </c>
       <c r="I6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" t="s">
         <v>34</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" t="s">
         <v>35</v>
       </c>
-      <c r="L6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>36</v>
       </c>
-      <c r="N6" t="s">
-        <v>37</v>
-      </c>
       <c r="O6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>48</v>
+      </c>
+      <c r="R6" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" t="s">
         <v>49</v>
       </c>
-      <c r="P6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>49</v>
-      </c>
-      <c r="R6" t="s">
-        <v>49</v>
-      </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>50</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
+        <v>38</v>
+      </c>
+      <c r="V6" t="s">
+        <v>41</v>
+      </c>
+      <c r="W6" t="s">
+        <v>92</v>
+      </c>
+      <c r="X6" t="s">
         <v>51</v>
       </c>
-      <c r="U6" t="s">
-        <v>39</v>
-      </c>
-      <c r="V6" t="s">
-        <v>42</v>
-      </c>
-      <c r="W6" t="s">
-        <v>93</v>
-      </c>
-      <c r="X6" t="s">
-        <v>52</v>
-      </c>
       <c r="Y6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AC6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
       <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
         <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
         <v>DURANT    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
         <v>31</v>
       </c>
-      <c r="H7" t="s">
-        <v>32</v>
-      </c>
       <c r="I7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" t="s">
         <v>34</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" t="s">
         <v>35</v>
       </c>
-      <c r="L7" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>36</v>
       </c>
-      <c r="N7" t="s">
-        <v>37</v>
-      </c>
       <c r="O7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P7" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>48</v>
+      </c>
+      <c r="R7" t="s">
+        <v>48</v>
+      </c>
+      <c r="S7" t="s">
         <v>49</v>
       </c>
-      <c r="P7" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>49</v>
-      </c>
-      <c r="R7" t="s">
-        <v>49</v>
-      </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>50</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
+        <v>38</v>
+      </c>
+      <c r="V7" t="s">
+        <v>41</v>
+      </c>
+      <c r="W7" t="s">
+        <v>93</v>
+      </c>
+      <c r="X7" t="s">
         <v>51</v>
       </c>
-      <c r="U7" t="s">
-        <v>39</v>
-      </c>
-      <c r="V7" t="s">
-        <v>42</v>
-      </c>
-      <c r="W7" t="s">
-        <v>94</v>
-      </c>
-      <c r="X7" t="s">
-        <v>52</v>
-      </c>
       <c r="Y7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AC7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
       <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" t="s">
         <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" t="s">
-        <v>47</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
         <v>DURANT    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
         <v>31</v>
       </c>
-      <c r="H8" t="s">
-        <v>32</v>
-      </c>
       <c r="I8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" t="s">
         <v>34</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" t="s">
         <v>35</v>
       </c>
-      <c r="L8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>36</v>
       </c>
-      <c r="N8" t="s">
-        <v>37</v>
-      </c>
       <c r="O8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P8" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>48</v>
+      </c>
+      <c r="R8" t="s">
+        <v>48</v>
+      </c>
+      <c r="S8" t="s">
         <v>49</v>
       </c>
-      <c r="P8" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>49</v>
-      </c>
-      <c r="R8" t="s">
-        <v>49</v>
-      </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>50</v>
       </c>
-      <c r="T8" t="s">
-        <v>51</v>
-      </c>
       <c r="U8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="X8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Y8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AC8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
       <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" t="s">
         <v>46</v>
-      </c>
-      <c r="D9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
         <v>DURANT    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
         <v>31</v>
       </c>
-      <c r="H9" t="s">
-        <v>32</v>
-      </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" t="s">
         <v>34</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" t="s">
         <v>35</v>
       </c>
-      <c r="L9" t="s">
-        <v>34</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>36</v>
       </c>
-      <c r="N9" t="s">
-        <v>37</v>
-      </c>
       <c r="O9" t="s">
+        <v>48</v>
+      </c>
+      <c r="P9" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>48</v>
+      </c>
+      <c r="R9" t="s">
+        <v>48</v>
+      </c>
+      <c r="S9" t="s">
         <v>49</v>
       </c>
-      <c r="P9" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>49</v>
-      </c>
-      <c r="R9" t="s">
-        <v>49</v>
-      </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>50</v>
       </c>
-      <c r="T9" t="s">
-        <v>51</v>
-      </c>
       <c r="U9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AC9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
       <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" t="s">
         <v>46</v>
-      </c>
-      <c r="D10" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" t="s">
-        <v>47</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
         <v>DURANT    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
         <v>31</v>
       </c>
-      <c r="H10" t="s">
-        <v>32</v>
-      </c>
       <c r="I10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" t="s">
         <v>34</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" t="s">
         <v>35</v>
       </c>
-      <c r="L10" t="s">
-        <v>34</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>36</v>
       </c>
-      <c r="N10" t="s">
-        <v>37</v>
-      </c>
       <c r="O10" t="s">
+        <v>48</v>
+      </c>
+      <c r="P10" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>48</v>
+      </c>
+      <c r="R10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S10" t="s">
         <v>49</v>
       </c>
-      <c r="P10" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>49</v>
-      </c>
-      <c r="R10" t="s">
-        <v>49</v>
-      </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>50</v>
       </c>
-      <c r="T10" t="s">
-        <v>51</v>
-      </c>
       <c r="U10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Y10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AC10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
       <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" t="s">
         <v>46</v>
-      </c>
-      <c r="D11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" t="s">
-        <v>47</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
         <v>DURANT    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" t="s">
         <v>31</v>
       </c>
-      <c r="H11" t="s">
-        <v>32</v>
-      </c>
       <c r="I11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" t="s">
         <v>34</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11" t="s">
         <v>35</v>
       </c>
-      <c r="L11" t="s">
-        <v>34</v>
-      </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>36</v>
       </c>
-      <c r="N11" t="s">
-        <v>37</v>
-      </c>
       <c r="O11" t="s">
+        <v>48</v>
+      </c>
+      <c r="P11" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>48</v>
+      </c>
+      <c r="R11" t="s">
+        <v>48</v>
+      </c>
+      <c r="S11" t="s">
         <v>49</v>
       </c>
-      <c r="P11" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>49</v>
-      </c>
-      <c r="R11" t="s">
-        <v>49</v>
-      </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>50</v>
       </c>
-      <c r="T11" t="s">
-        <v>51</v>
-      </c>
       <c r="U11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="X11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Y11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
       <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" t="s">
         <v>46</v>
-      </c>
-      <c r="D12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
         <v>DURANT    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" t="s">
         <v>31</v>
       </c>
-      <c r="H12" t="s">
-        <v>32</v>
-      </c>
       <c r="I12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" t="s">
         <v>34</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" t="s">
         <v>35</v>
       </c>
-      <c r="L12" t="s">
-        <v>34</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>36</v>
       </c>
-      <c r="N12" t="s">
-        <v>37</v>
-      </c>
       <c r="O12" t="s">
+        <v>48</v>
+      </c>
+      <c r="P12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>48</v>
+      </c>
+      <c r="R12" t="s">
+        <v>48</v>
+      </c>
+      <c r="S12" t="s">
         <v>49</v>
       </c>
-      <c r="P12" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>49</v>
-      </c>
-      <c r="R12" t="s">
-        <v>49</v>
-      </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>50</v>
       </c>
-      <c r="T12" t="s">
-        <v>51</v>
-      </c>
       <c r="U12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Y12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
       <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" t="s">
         <v>46</v>
-      </c>
-      <c r="D13" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" t="s">
-        <v>47</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
         <v>DURANT    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
         <v>31</v>
       </c>
-      <c r="H13" t="s">
-        <v>32</v>
-      </c>
       <c r="I13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" t="s">
         <v>34</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" t="s">
         <v>35</v>
       </c>
-      <c r="L13" t="s">
-        <v>34</v>
-      </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>36</v>
       </c>
-      <c r="N13" t="s">
-        <v>37</v>
-      </c>
       <c r="O13" t="s">
+        <v>48</v>
+      </c>
+      <c r="P13" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>48</v>
+      </c>
+      <c r="R13" t="s">
+        <v>48</v>
+      </c>
+      <c r="S13" t="s">
         <v>49</v>
       </c>
-      <c r="P13" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>49</v>
-      </c>
-      <c r="R13" t="s">
-        <v>49</v>
-      </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>50</v>
       </c>
-      <c r="T13" t="s">
-        <v>51</v>
-      </c>
       <c r="U13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="X13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Y13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
       <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" t="s">
         <v>46</v>
-      </c>
-      <c r="D14" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" t="s">
-        <v>47</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
         <v>DURANT    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" t="s">
         <v>31</v>
       </c>
-      <c r="H14" t="s">
-        <v>32</v>
-      </c>
       <c r="I14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" t="s">
         <v>34</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
+        <v>33</v>
+      </c>
+      <c r="M14" t="s">
         <v>35</v>
       </c>
-      <c r="L14" t="s">
-        <v>34</v>
-      </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>36</v>
       </c>
-      <c r="N14" t="s">
-        <v>37</v>
-      </c>
       <c r="O14" t="s">
+        <v>48</v>
+      </c>
+      <c r="P14" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>48</v>
+      </c>
+      <c r="R14" t="s">
+        <v>48</v>
+      </c>
+      <c r="S14" t="s">
         <v>49</v>
       </c>
-      <c r="P14" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>49</v>
-      </c>
-      <c r="R14" t="s">
-        <v>49</v>
-      </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>50</v>
       </c>
-      <c r="T14" t="s">
-        <v>51</v>
-      </c>
       <c r="U14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W14" t="s">
+        <v>56</v>
+      </c>
+      <c r="X14" t="s">
         <v>57</v>
       </c>
-      <c r="X14" t="s">
-        <v>58</v>
-      </c>
       <c r="Y14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AC14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
       <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" t="s">
         <v>59</v>
-      </c>
-      <c r="D15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" t="s">
-        <v>60</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
         <v>DUPOND    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" t="s">
         <v>31</v>
       </c>
-      <c r="H15" t="s">
-        <v>32</v>
-      </c>
       <c r="I15" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" t="s">
+        <v>34</v>
+      </c>
+      <c r="L15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M15" t="s">
+        <v>35</v>
+      </c>
+      <c r="N15" t="s">
+        <v>36</v>
+      </c>
+      <c r="O15" t="s">
         <v>61</v>
       </c>
-      <c r="J15" t="s">
-        <v>34</v>
-      </c>
-      <c r="K15" t="s">
-        <v>35</v>
-      </c>
-      <c r="L15" t="s">
-        <v>34</v>
-      </c>
-      <c r="M15" t="s">
-        <v>36</v>
-      </c>
-      <c r="N15" t="s">
-        <v>37</v>
-      </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>61</v>
+      </c>
+      <c r="R15" t="s">
+        <v>61</v>
+      </c>
+      <c r="S15" t="s">
+        <v>39</v>
+      </c>
+      <c r="T15" t="s">
         <v>62</v>
       </c>
-      <c r="P15" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>62</v>
-      </c>
-      <c r="R15" t="s">
-        <v>62</v>
-      </c>
-      <c r="S15" t="s">
-        <v>40</v>
-      </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
+        <v>38</v>
+      </c>
+      <c r="V15" t="s">
+        <v>41</v>
+      </c>
+      <c r="W15" t="s">
+        <v>99</v>
+      </c>
+      <c r="X15" t="s">
         <v>63</v>
       </c>
-      <c r="U15" t="s">
-        <v>39</v>
-      </c>
-      <c r="V15" t="s">
-        <v>42</v>
-      </c>
-      <c r="W15" t="s">
-        <v>100</v>
-      </c>
-      <c r="X15" t="s">
-        <v>64</v>
-      </c>
       <c r="Y15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AC15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
       <c r="C16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" t="s">
         <v>59</v>
-      </c>
-      <c r="D16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" t="s">
-        <v>60</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
         <v>DUPOND    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" t="s">
         <v>31</v>
       </c>
-      <c r="H16" t="s">
-        <v>32</v>
-      </c>
       <c r="I16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16" t="s">
+        <v>35</v>
+      </c>
+      <c r="N16" t="s">
+        <v>36</v>
+      </c>
+      <c r="O16" t="s">
         <v>61</v>
       </c>
-      <c r="J16" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" t="s">
-        <v>35</v>
-      </c>
-      <c r="L16" t="s">
-        <v>34</v>
-      </c>
-      <c r="M16" t="s">
-        <v>36</v>
-      </c>
-      <c r="N16" t="s">
-        <v>37</v>
-      </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>61</v>
+      </c>
+      <c r="R16" t="s">
+        <v>61</v>
+      </c>
+      <c r="S16" t="s">
+        <v>39</v>
+      </c>
+      <c r="T16" t="s">
         <v>62</v>
       </c>
-      <c r="P16" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>62</v>
-      </c>
-      <c r="R16" t="s">
-        <v>62</v>
-      </c>
-      <c r="S16" t="s">
-        <v>40</v>
-      </c>
-      <c r="T16" t="s">
-        <v>63</v>
-      </c>
       <c r="U16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Y16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AC16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
         <v>27</v>
       </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
       <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" t="s">
         <v>59</v>
-      </c>
-      <c r="D17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" t="s">
-        <v>60</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
         <v>DUPOND    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" t="s">
         <v>31</v>
       </c>
-      <c r="H17" t="s">
-        <v>32</v>
-      </c>
       <c r="I17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" t="s">
+        <v>34</v>
+      </c>
+      <c r="L17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" t="s">
+        <v>35</v>
+      </c>
+      <c r="N17" t="s">
+        <v>36</v>
+      </c>
+      <c r="O17" t="s">
         <v>61</v>
       </c>
-      <c r="J17" t="s">
-        <v>34</v>
-      </c>
-      <c r="K17" t="s">
-        <v>35</v>
-      </c>
-      <c r="L17" t="s">
-        <v>34</v>
-      </c>
-      <c r="M17" t="s">
-        <v>36</v>
-      </c>
-      <c r="N17" t="s">
-        <v>37</v>
-      </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>61</v>
+      </c>
+      <c r="R17" t="s">
+        <v>61</v>
+      </c>
+      <c r="S17" t="s">
+        <v>39</v>
+      </c>
+      <c r="T17" t="s">
         <v>62</v>
       </c>
-      <c r="P17" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>62</v>
-      </c>
-      <c r="R17" t="s">
-        <v>62</v>
-      </c>
-      <c r="S17" t="s">
-        <v>40</v>
-      </c>
-      <c r="T17" t="s">
-        <v>63</v>
-      </c>
       <c r="U17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="X17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Y17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AC17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
       <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" t="s">
         <v>59</v>
-      </c>
-      <c r="D18" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" t="s">
-        <v>60</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
         <v>DUPOND    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" t="s">
         <v>31</v>
       </c>
-      <c r="H18" t="s">
-        <v>32</v>
-      </c>
       <c r="I18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" t="s">
+        <v>35</v>
+      </c>
+      <c r="N18" t="s">
+        <v>36</v>
+      </c>
+      <c r="O18" t="s">
         <v>61</v>
       </c>
-      <c r="J18" t="s">
-        <v>34</v>
-      </c>
-      <c r="K18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L18" t="s">
-        <v>34</v>
-      </c>
-      <c r="M18" t="s">
-        <v>36</v>
-      </c>
-      <c r="N18" t="s">
-        <v>37</v>
-      </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>61</v>
+      </c>
+      <c r="R18" t="s">
+        <v>61</v>
+      </c>
+      <c r="S18" t="s">
+        <v>39</v>
+      </c>
+      <c r="T18" t="s">
         <v>62</v>
       </c>
-      <c r="P18" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>62</v>
-      </c>
-      <c r="R18" t="s">
-        <v>62</v>
-      </c>
-      <c r="S18" t="s">
-        <v>40</v>
-      </c>
-      <c r="T18" t="s">
-        <v>63</v>
-      </c>
       <c r="U18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="X18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Y18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AC18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
         <v>27</v>
       </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
       <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" t="s">
         <v>66</v>
-      </c>
-      <c r="D19" t="s">
-        <v>87</v>
-      </c>
-      <c r="E19" t="s">
-        <v>67</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
         <v>DURAND    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" t="s">
         <v>31</v>
       </c>
-      <c r="H19" t="s">
-        <v>32</v>
-      </c>
       <c r="I19" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19" t="s">
+        <v>33</v>
+      </c>
+      <c r="M19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O19" t="s">
         <v>68</v>
       </c>
-      <c r="J19" t="s">
-        <v>34</v>
-      </c>
-      <c r="K19" t="s">
-        <v>35</v>
-      </c>
-      <c r="L19" t="s">
-        <v>34</v>
-      </c>
-      <c r="M19" t="s">
-        <v>36</v>
-      </c>
-      <c r="N19" t="s">
-        <v>37</v>
-      </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>68</v>
+      </c>
+      <c r="R19" t="s">
+        <v>68</v>
+      </c>
+      <c r="S19" t="s">
+        <v>49</v>
+      </c>
+      <c r="T19" t="s">
         <v>69</v>
       </c>
-      <c r="P19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>69</v>
-      </c>
-      <c r="R19" t="s">
-        <v>69</v>
-      </c>
-      <c r="S19" t="s">
-        <v>50</v>
-      </c>
-      <c r="T19" t="s">
-        <v>70</v>
-      </c>
       <c r="U19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="X19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Y19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AC19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
         <v>27</v>
       </c>
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
       <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" t="s">
         <v>66</v>
-      </c>
-      <c r="D20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E20" t="s">
-        <v>67</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
         <v>DURAND    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" t="s">
         <v>31</v>
       </c>
-      <c r="H20" t="s">
-        <v>32</v>
-      </c>
       <c r="I20" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" t="s">
+        <v>34</v>
+      </c>
+      <c r="L20" t="s">
+        <v>33</v>
+      </c>
+      <c r="M20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N20" t="s">
+        <v>36</v>
+      </c>
+      <c r="O20" t="s">
         <v>68</v>
       </c>
-      <c r="J20" t="s">
-        <v>34</v>
-      </c>
-      <c r="K20" t="s">
-        <v>35</v>
-      </c>
-      <c r="L20" t="s">
-        <v>34</v>
-      </c>
-      <c r="M20" t="s">
-        <v>36</v>
-      </c>
-      <c r="N20" t="s">
-        <v>37</v>
-      </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>68</v>
+      </c>
+      <c r="R20" t="s">
+        <v>68</v>
+      </c>
+      <c r="S20" t="s">
+        <v>49</v>
+      </c>
+      <c r="T20" t="s">
         <v>69</v>
       </c>
-      <c r="P20" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>69</v>
-      </c>
-      <c r="R20" t="s">
-        <v>69</v>
-      </c>
-      <c r="S20" t="s">
-        <v>50</v>
-      </c>
-      <c r="T20" t="s">
-        <v>70</v>
-      </c>
       <c r="U20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="X20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Y20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AC20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
         <v>27</v>
       </c>
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
       <c r="C21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" t="s">
         <v>66</v>
-      </c>
-      <c r="D21" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" t="s">
-        <v>67</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
         <v>DURAND    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" t="s">
         <v>31</v>
       </c>
-      <c r="H21" t="s">
-        <v>32</v>
-      </c>
       <c r="I21" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" t="s">
+        <v>33</v>
+      </c>
+      <c r="K21" t="s">
+        <v>34</v>
+      </c>
+      <c r="L21" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21" t="s">
+        <v>35</v>
+      </c>
+      <c r="N21" t="s">
+        <v>36</v>
+      </c>
+      <c r="O21" t="s">
         <v>68</v>
       </c>
-      <c r="J21" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21" t="s">
-        <v>35</v>
-      </c>
-      <c r="L21" t="s">
-        <v>34</v>
-      </c>
-      <c r="M21" t="s">
-        <v>36</v>
-      </c>
-      <c r="N21" t="s">
-        <v>37</v>
-      </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>68</v>
+      </c>
+      <c r="R21" t="s">
+        <v>68</v>
+      </c>
+      <c r="S21" t="s">
+        <v>49</v>
+      </c>
+      <c r="T21" t="s">
         <v>69</v>
       </c>
-      <c r="P21" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>69</v>
-      </c>
-      <c r="R21" t="s">
-        <v>69</v>
-      </c>
-      <c r="S21" t="s">
-        <v>50</v>
-      </c>
-      <c r="T21" t="s">
-        <v>70</v>
-      </c>
       <c r="U21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Y21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
         <v>27</v>
       </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
       <c r="C22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" t="s">
         <v>71</v>
-      </c>
-      <c r="D22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" t="s">
-        <v>72</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
         <v>DEMO    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" t="s">
         <v>31</v>
       </c>
-      <c r="H22" t="s">
-        <v>32</v>
-      </c>
       <c r="I22" t="s">
+        <v>72</v>
+      </c>
+      <c r="J22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22" t="s">
+        <v>34</v>
+      </c>
+      <c r="L22" t="s">
+        <v>33</v>
+      </c>
+      <c r="M22" t="s">
+        <v>35</v>
+      </c>
+      <c r="N22" t="s">
+        <v>36</v>
+      </c>
+      <c r="O22" t="s">
         <v>73</v>
       </c>
-      <c r="J22" t="s">
-        <v>34</v>
-      </c>
-      <c r="K22" t="s">
-        <v>35</v>
-      </c>
-      <c r="L22" t="s">
-        <v>34</v>
-      </c>
-      <c r="M22" t="s">
-        <v>36</v>
-      </c>
-      <c r="N22" t="s">
-        <v>37</v>
-      </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>73</v>
+      </c>
+      <c r="R22" t="s">
+        <v>73</v>
+      </c>
+      <c r="S22" t="s">
         <v>74</v>
       </c>
-      <c r="P22" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>74</v>
-      </c>
-      <c r="R22" t="s">
-        <v>74</v>
-      </c>
-      <c r="S22" t="s">
+      <c r="T22" t="s">
         <v>75</v>
       </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
+        <v>38</v>
+      </c>
+      <c r="V22" t="s">
+        <v>41</v>
+      </c>
+      <c r="W22" t="s">
+        <v>105</v>
+      </c>
+      <c r="X22" t="s">
         <v>76</v>
       </c>
-      <c r="U22" t="s">
-        <v>39</v>
-      </c>
-      <c r="V22" t="s">
-        <v>42</v>
-      </c>
-      <c r="W22" t="s">
-        <v>106</v>
-      </c>
-      <c r="X22" t="s">
-        <v>77</v>
-      </c>
       <c r="Y22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AC22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" t="s">
-        <v>28</v>
-      </c>
       <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" t="s">
         <v>71</v>
-      </c>
-      <c r="D23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" t="s">
-        <v>72</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
         <v>DEMO    Chaussée de Ruisbroek 18  1180 Uccle Belgique</v>
       </c>
       <c r="G23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" t="s">
         <v>31</v>
       </c>
-      <c r="H23" t="s">
-        <v>32</v>
-      </c>
       <c r="I23" t="s">
+        <v>72</v>
+      </c>
+      <c r="J23" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" t="s">
+        <v>34</v>
+      </c>
+      <c r="L23" t="s">
+        <v>33</v>
+      </c>
+      <c r="M23" t="s">
+        <v>35</v>
+      </c>
+      <c r="N23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O23" t="s">
         <v>73</v>
       </c>
-      <c r="J23" t="s">
-        <v>34</v>
-      </c>
-      <c r="K23" t="s">
-        <v>35</v>
-      </c>
-      <c r="L23" t="s">
-        <v>34</v>
-      </c>
-      <c r="M23" t="s">
-        <v>36</v>
-      </c>
-      <c r="N23" t="s">
-        <v>37</v>
-      </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>73</v>
+      </c>
+      <c r="R23" t="s">
+        <v>73</v>
+      </c>
+      <c r="S23" t="s">
         <v>74</v>
       </c>
-      <c r="P23" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>74</v>
-      </c>
-      <c r="R23" t="s">
-        <v>74</v>
-      </c>
-      <c r="S23" t="s">
+      <c r="T23" t="s">
         <v>75</v>
       </c>
-      <c r="T23" t="s">
-        <v>76</v>
-      </c>
       <c r="U23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Y23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AC23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>